<commit_message>
parts updated for LCSC orders
</commit_message>
<xml_diff>
--- a/_OUTPUT/BOM.xlsx
+++ b/_OUTPUT/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angrypig\Angrypig\Dev\LoRa_Transmitter\LoRa_Shield\_OUTPUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7DF1DF45-705D-4263-BA85-F08852CEF833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7EE49D47-04E1-485B-A4B0-2B7060F0396F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM." localSheetId="0">BOM!$A$1:$D$24</definedName>
+    <definedName name="BOM." localSheetId="0">BOM!$A$1:$B$24</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
   <si>
     <t>Device</t>
   </si>
@@ -65,9 +65,6 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C-EUC0603</t>
-  </si>
-  <si>
     <t>C0603</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>22uF</t>
   </si>
   <si>
-    <t>C-EUC0805</t>
-  </si>
-  <si>
     <t>C0805</t>
   </si>
   <si>
@@ -89,193 +83,236 @@
     <t>100uF</t>
   </si>
   <si>
-    <t>CPOL-USSMCB</t>
-  </si>
-  <si>
-    <t>SMC_B</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
     <t>B5819W</t>
   </si>
   <si>
+    <t>SOD-123</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>BAT54SWT1G</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>AHT10</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>TXS0102DCUR</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>TYPE-C-31-M-17</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CON_TERMINAL_BLOCK_03-5MM</t>
+  </si>
+  <si>
+    <t>TERMINAL_BLOCK_3P_5</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>JP5</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>JP8</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>RFM98W</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>BU-SMA-H</t>
+  </si>
+  <si>
+    <t>C1, C3, C4, C5, C6, C7, C9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JP4, JP7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1, R3, R5, R6, R8, R10, R12</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>R7, R9, R11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>165k (0,1%)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15k (0.1%)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3V Regulator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Designator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header, 0.254mm, 2x1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header, 0.254mm, 4x1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header, 0.254mm, 8x1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header, 0.254mm, 10x1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header, 0.254mm, 6x1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Header, 0.254mm, 3x1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RFM98W</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>DIODE-SOD-123</t>
-  </si>
-  <si>
-    <t>SOD-123</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>BAT54SWT1G</t>
-  </si>
-  <si>
-    <t>SOT65P220X100-3N</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>AHT10</t>
-  </si>
-  <si>
-    <t>IC2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMC-B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>C_0603</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>C_0805</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>C_SMC-B</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_0603</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOT-323(SC-70)</t>
   </si>
   <si>
     <t>TXS0102DCUR</t>
-  </si>
-  <si>
-    <t>SOP50P310X90-8N</t>
-  </si>
-  <si>
-    <t>J1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>US8</t>
   </si>
   <si>
     <t>TYPE-C-31-M-17</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>CON_TERMINAL_BLOCK_03-5MM</t>
-  </si>
-  <si>
-    <t>TERMINAL_BLOCK_3P_5</t>
-  </si>
-  <si>
-    <t>JP2</t>
-  </si>
-  <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>JP5</t>
-  </si>
-  <si>
-    <t>JP6</t>
-  </si>
-  <si>
-    <t>JP8</t>
-  </si>
-  <si>
-    <t>LED1</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>LEDCHIP-LED0603</t>
-  </si>
-  <si>
-    <t>CHIP-LED0603</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R-US_R0603</t>
-  </si>
-  <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>5k</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>AZ1117H-5.0TRE1</t>
-  </si>
-  <si>
-    <t>SOT230P700X170-4N</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>RFM98W</t>
-  </si>
-  <si>
-    <t>RFM95W</t>
-  </si>
-  <si>
-    <t>RFM95/96/97/98W</t>
-  </si>
-  <si>
-    <t>X1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>BU-SMA-H</t>
-  </si>
-  <si>
-    <t>C1, C3, C4, C5, C6, C7, C9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>JP4, JP7</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1, R3, R5, R6, R8, R10, R12</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>R7, R9, R11</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>165k (0,1%)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>15k (0.1%)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.3V Regulator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Designator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header, 0.254mm, 2x1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header, 0.254mm, 4x1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header, 0.254mm, 8x1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header, 0.254mm, 10x1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header, 0.254mm, 6x1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Header, 0.254mm, 3x1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCSC Part #</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>C22809</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>C45783</t>
+  </si>
+  <si>
+    <t>C14663</t>
+  </si>
+  <si>
+    <t>C16133</t>
+  </si>
+  <si>
+    <t>C95612</t>
+  </si>
+  <si>
+    <t>LED0803</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED_0805</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOT-23-3L</t>
+  </si>
+  <si>
+    <t>XC6206P332MR</t>
   </si>
 </sst>
 </file>
@@ -1234,340 +1271,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
         <v>65</v>
       </c>
-      <c r="D13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D24">
+  <sortState ref="A2:B24">
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
schematic resistor value, arduino code
</commit_message>
<xml_diff>
--- a/_OUTPUT/BOM.xlsx
+++ b/_OUTPUT/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angrypig\Angrypig\Dev\LoRa_Transmitter\LoRa_Shield\_OUTPUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D78912-DBBA-4726-8EE9-6072891BBC94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7119D9-A912-46AF-83B2-321256E1CF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>Device</t>
   </si>
@@ -193,14 +193,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>165k (0,1%)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>15k (0.1%)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>3.3V Regulator</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -286,9 +278,6 @@
     <t>C25804</t>
   </si>
   <si>
-    <t>C95612</t>
-  </si>
-  <si>
     <t>LED_0805</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -306,10 +295,6 @@
     <t>DFN-6</t>
   </si>
   <si>
-    <t>C22809</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>C23162</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -366,6 +351,14 @@
   </si>
   <si>
     <t>C411575</t>
+  </si>
+  <si>
+    <t>110k (0,1%)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10k (0.1%)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1326,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1340,7 +1333,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1352,7 +1345,7 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1363,13 +1356,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1380,13 +1373,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1394,16 +1387,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1414,13 +1407,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1428,7 +1421,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1445,16 +1438,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1462,13 +1455,13 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
@@ -1479,7 +1472,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1488,7 +1481,7 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1496,16 +1489,16 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1513,10 +1506,10 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1524,10 +1517,10 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1535,10 +1528,10 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1546,10 +1539,10 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1557,10 +1550,10 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,10 +1561,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1579,13 +1572,13 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1596,13 +1589,13 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
         <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1613,13 +1606,13 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1630,13 +1623,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1647,13 +1637,10 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1661,16 +1648,16 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1678,16 +1665,16 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1695,7 +1682,7 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -1704,7 +1691,7 @@
         <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>